<commit_message>
fix db user creadential
</commit_message>
<xml_diff>
--- a/uploads/data/contoh_format_excel.xlsx
+++ b/uploads/data/contoh_format_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anonimox\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\keuangan\uploads\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1913ED27-260B-4A56-AF2A-58B2D371A236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2FE05E-8B2B-453B-A74E-94C8F0FCB808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0EA281BF-02DB-492B-900F-DF763AB3E8E2}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>NIS</t>
   </si>
@@ -64,6 +64,73 @@
     <t>08977665544</t>
   </si>
   <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SMP</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>DAISAH</t>
+  </si>
+  <si>
+    <t>HISYAH</t>
+  </si>
+  <si>
+    <t>08977665546</t>
+  </si>
+  <si>
+    <t>08977665548</t>
+  </si>
+  <si>
+    <t>AHRA AHIA</t>
+  </si>
+  <si>
+    <t>RASHA</t>
+  </si>
+  <si>
+    <t>KYAHRA SHAHIA ZURAFA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*untuk format isian kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NIS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wajib maksimal 5-7 karakter angka </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>*untuk format isian kolom</t>
     </r>
@@ -76,41 +143,63 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> NOMOR _HP_WALI  wajib menggunkan "0" bukan "+62"</t>
-    </r>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>SMP</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>BAISAH</t>
-  </si>
-  <si>
-    <t>CISYAH</t>
-  </si>
-  <si>
-    <t>DAISAH</t>
-  </si>
-  <si>
-    <t>HISYAH</t>
-  </si>
-  <si>
-    <t>08977665545</t>
-  </si>
-  <si>
-    <t>08977665546</t>
-  </si>
-  <si>
-    <t>08977665547</t>
-  </si>
-  <si>
-    <t>08977665548</t>
+      <t xml:space="preserve"> SALDO UMUM/QURBAN/WISATA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wajib diisi minimal 0 rupiah &amp; tanpa koma/titik</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*untuk format isian kolom</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NAMA_WALI, NOMOR_HP_WALI, EMAIL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tidak wajib di isi, "kosongkan" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(TIDAK WAJIB DI ISI)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -125,7 +214,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NIS</t>
+      <t>TINGKAT</t>
     </r>
     <r>
       <rPr>
@@ -135,7 +224,55 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> wajib maksimal 5-6 karakter angka</t>
+      <t xml:space="preserve"> wajib (DC/KB/TK/SD/SMP)  tanpa ICP dll </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <r>
+      <t>*untuk format isian kolom</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NOMOR _HP_WALI  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wajib menggunkan "0" bukan "+62" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(TIDAK WAJIB DI ISI)</t>
     </r>
   </si>
   <si>
@@ -151,7 +288,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>TINGKAT</t>
+      <t>NAMA</t>
     </r>
     <r>
       <rPr>
@@ -161,24 +298,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> wajib (KB/TK/SD/SMP)  tanpa ICP dll</t>
-    </r>
-  </si>
-  <si>
-    <t>AHRA AHIA</t>
-  </si>
-  <si>
-    <t>KYA SHA</t>
-  </si>
-  <si>
-    <t>RASHA</t>
-  </si>
-  <si>
-    <t>KYAHRA SHAHIA ZURAFA</t>
-  </si>
-  <si>
-    <r>
-      <t>*untuk format isian kolom</t>
+      <t xml:space="preserve"> gunakan karakter biasa </t>
     </r>
     <r>
       <rPr>
@@ -189,17 +309,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> SALDO UMUM/QURBAN/WISATA WAJIB DIISI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>minimal 0 rupiah &amp; tanpa koma/titik</t>
+      <t>(WAJIB DI ISI)</t>
     </r>
   </si>
 </sst>
@@ -207,7 +317,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +489,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -725,12 +848,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1108,13 +1233,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA0F0B5-3F2A-41A4-B914-484C0C045741}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L10" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -1123,17 +1248,17 @@
     <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="88.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="104.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -1145,13 +1270,13 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1160,7 +1285,7 @@
         <v>123456</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1186,115 +1311,112 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>123457</v>
+        <v>123458</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3">
-        <v>100000</v>
+        <v>300000</v>
       </c>
       <c r="H3">
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="I3">
-        <v>100000</v>
+        <v>400000</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>123458</v>
+        <v>123459</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
       <c r="G4">
-        <v>300000</v>
+        <v>500000</v>
       </c>
       <c r="H4">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>400000</v>
+        <v>700000</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>123459</v>
+        <v>123460</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5">
+        <v>700000</v>
+      </c>
+      <c r="H5">
+        <v>500000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5">
-        <v>500000</v>
-      </c>
-      <c r="H5">
-        <v>400000</v>
-      </c>
-      <c r="I5">
-        <v>700000</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>123460</v>
+        <v>1234666</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6">
-        <v>700000</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1303,17 +1425,35 @@
         <v>1000000</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L7" s="2" t="s">
-        <v>32</v>
+      <c r="A7">
+        <v>1234666</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L8" s="2" t="s">
-        <v>14</v>
+      <c r="L8" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix role for saving
</commit_message>
<xml_diff>
--- a/uploads/data/contoh_format_excel.xlsx
+++ b/uploads/data/contoh_format_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\keuangan\uploads\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2FE05E-8B2B-453B-A74E-94C8F0FCB808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD3A85-0C15-463F-9298-BC6267605058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0EA281BF-02DB-492B-900F-DF763AB3E8E2}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>NIS</t>
   </si>
@@ -310,6 +310,52 @@
         <scheme val="minor"/>
       </rPr>
       <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <t>STATUS_SISWA</t>
+  </si>
+  <si>
+    <t>TIDAK AKTIF</t>
+  </si>
+  <si>
+    <t>AKTIF</t>
+  </si>
+  <si>
+    <r>
+      <t>*untuk format isian kolom</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> STATUS_SISWA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wajib diisi (TIDAK AKTIF/AKTIF)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (WAJIB DI ISI)</t>
     </r>
   </si>
 </sst>
@@ -848,14 +894,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1231,228 +1292,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA0F0B5-3F2A-41A4-B914-484C0C045741}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="104.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="12" max="12" width="98.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>123456</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>200000</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>100000</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>300000</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>123458</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>300000</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>300000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>400000</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="J3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>123459</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>500000</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>700000</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="J4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>123460</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>700000</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>500000</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>0</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="J5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>1234666</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>500000</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>1000000</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>1234666</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>0</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>29</v>
+      <c r="J7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L9" s="7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>